<commit_message>
Excel files summarized for John. 'Taxa names' created based on raw files outside this folder. May need to be updated.
</commit_message>
<xml_diff>
--- a/Sostrpro2018_Invert_density_summary.xlsx
+++ b/Sostrpro2018_Invert_density_summary.xlsx
@@ -1095,7 +1095,7 @@
   <dimension ref="A1:DF13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection sqref="A1:DF1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5426,7 +5426,7 @@
   <dimension ref="A1:EH13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>